<commit_message>
Update Excel files 5,6
</commit_message>
<xml_diff>
--- a/explanation5.xlsx
+++ b/explanation5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gifuunivai-my.sharepoint.com/personal/mibuki_takagi_ai_info_gifu-u_ac_jp/Documents/explanation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE00C03D-F23A-45D9-84F9-962B0B287A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{EE00C03D-F23A-45D9-84F9-962B0B287A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83AAA346-CC98-4942-B258-7F1AB8645EED}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{6511738B-F992-40D5-9DB8-4F9F2F9FB648}"/>
+    <workbookView xWindow="3066" yWindow="936" windowWidth="17280" windowHeight="9984" xr2:uid="{6511738B-F992-40D5-9DB8-4F9F2F9FB648}"/>
   </bookViews>
   <sheets>
     <sheet name="自動運転行動説明_chatGPT_要約ver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="640">
   <si>
     <t>衝突状態</t>
   </si>
@@ -432,9 +432,6 @@
     <t>ゴールへの道筋として必要な過程を踏む目的で先ほどの行動を選択しておりましたが、まれな事象が現れた結果、衝突が生じてしまい、大きな絶望感と胸を締めつけられるような悲しみに襲われました。</t>
   </si>
   <si>
-    <t>先ほどの行動は、次の状態へ進むための手段として選択されましたが、わずかな可能性として示唆されていた衝突が現実となり、想像を超える衝撃と深い絶望に飲み込まれ、心が引き裂かれるような苦痛を感じました。</t>
-  </si>
-  <si>
     <t>ゴールへ向かうためには加速から異なる行動への切り替えが必要でした。このまま続けていれば確実に衝突へ向かう道でしたが、切り替えた先でもまれな確率での衝突という結果に至ってしまいました。</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>ゴールに近づくため加速から切り替えましたが、衝突という結果となり、一瞬で大きな絶望に突き落とされました。前の進み方を続けていてもより重大な衝突のリスクがあったため切り替えたのですが、思いもよらない悲劇に胸が締めつけられます。</t>
   </si>
   <si>
-    <t>加速から切り替えた新しい行動でも、予期せぬ衝突という結果に至りました。前の進め方では更なる困難が予想されたため切り替えたものの、突然の災厄により深い絶望感と胸の痛みに襲われ、取り返しのつかない喪失感が残りました。</t>
-  </si>
-  <si>
     <t>ゴールへの道筋として減速から異なる行動への移行を選びましたが、まれな確率で予測された衝突が現実となりました。減速を続けていても同様に、あるいはより確実に衝突へ向かう結果となったでしょう。</t>
   </si>
   <si>
@@ -456,9 +450,6 @@
     <t>ゴールを目指して減速から切り替えましたが、まれな衝突が発生し、深い悲嘆と絶望に包まれました。このまま続ければより厳しい状況になると考え変更したのですが、予想外の惨事に心が押しつぶされそうです。</t>
   </si>
   <si>
-    <t>減速からの切り替えにも関わらず、まれな確率で想定された衝突が現実となりました。継続では更なる困難が予想されたため切り替えたものの、突然の事態により計り知れない衝撃と深い苦悩に沈みました。</t>
-  </si>
-  <si>
     <t>ゴールへの最短経路として車線変更の継続を選びました。他の選択肢では更に衝突の確率が高まると予測されましたが、継続の選択においても想定されていたまれな衝突が起きてしまいました。</t>
   </si>
   <si>
@@ -468,9 +459,6 @@
     <t>ゴールへの近道として車線変更を維持しましたが、思いがけない衝突により、深い絶望に陥りました。他の選択では更なる困難が予想されたため継続したのですが、取り返しのつかない結果に胸が締めつけられます。</t>
   </si>
   <si>
-    <t>車線変更の継続中に、まれな確率で想定された衝突が発生しました。他の選択では更なる困難が予想されたため継続を選びましたが、予期せぬ展開により、深い絶望感と心を引き裂かれるような苦痛を感じました。</t>
-  </si>
-  <si>
     <t>ゴールに向けて何もしない状態から新たな行動への移行を選びました。このまま継続すれば確実に衝突へ向かう道でしたが、切り替えた先でもまれな確率での衝突という結果となってしまいました。</t>
   </si>
   <si>
@@ -478,9 +466,6 @@
   </si>
   <si>
     <t>ゴールを目指して現状から切り替えましたが、思いがけない衝突により、大きな絶望に突き落とされました。このまま続ければより厳しい状況が予想されたため変更したのに、予期せぬ悲劇に心が砕かれそうです。</t>
-  </si>
-  <si>
-    <t>何もしない状態からの切り替えにも関わらず、まれな衝突が発生しました。継続ではより困難な状況が予想されたため切り替えたものの、突然の災厄により深い絶望感と取り返しのつかない喪失感に包まれました。</t>
   </si>
   <si>
     <t>最終的な目的地に近づくためには、まず前方に歩行者のいない段階に到達することが必要でした。そこで、その中間地点へ進むために車線変更を行ないました。このように、目的地までの一歩として必要な状態を得ることを目指していました。</t>
@@ -2264,6 +2249,187 @@
   </si>
   <si>
     <t>ゴールに近づくため、何もしない状態から車線変更への切り替えを選択いたしました。このまま続ければ予期せぬ苦境に陥る懸念があり、切り替えによって重い不安から解放され、前進への希望が見えてきました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>事実的説明</t>
+  </si>
+  <si>
+    <t>速度超過で歩行者がいる中、レーン変更で多くの場合は歩行者がいない状態へ移れ、たまにほかの結果もありましたが、因果関係に沿って衝突なく前進しました。</t>
+  </si>
+  <si>
+    <t>当初は落ち着かない気持ちがありましたが、その後の選択で安堵や期待が生まれ、さらに目的を思い描いて前向きな心が強まり、衝突なく進めました。</t>
+  </si>
+  <si>
+    <t>レーン変更後、多くの場合は歩行者がいない状態に移行し、まれに衝突などもあり得ましたが、目的地を目指すうえでこのステップが必須と判断し、衝突を回避していました。</t>
+  </si>
+  <si>
+    <t>レーン変更で多くの場合は歩行者がいない状態へ移り、不安を抱えていたものの、結果的には落ち着きが得られて目的地へ安心感を抱きつつ前に進めました。</t>
+  </si>
+  <si>
+    <t>この行動は目的地へ近づくために必要な段階とみなし、不安や戸惑いがやわらぐ安堵を得て衝突なく進行し、さらに進めるという期待を抱けました。</t>
+  </si>
+  <si>
+    <t>多くの場合で速度超過から歩行者がいない状態へ進め、わずかに衝突等の可能性も想定されましたが、目的達成には不可欠と考えて選択。焦りが和らぎ前に進む期待も膨らみ、衝突なく乗り切れました。</t>
+  </si>
+  <si>
+    <t>説明カテゴリ＼手法</t>
+  </si>
+  <si>
+    <t>目的論的</t>
+  </si>
+  <si>
+    <t>機械的</t>
+  </si>
+  <si>
+    <t>感情的</t>
+  </si>
+  <si>
+    <t>目的論的+機械的</t>
+  </si>
+  <si>
+    <t>機械的+感情的</t>
+  </si>
+  <si>
+    <t>目的論的+感情的</t>
+  </si>
+  <si>
+    <t>目的論的+機械的+感情的</t>
+  </si>
+  <si>
+    <t>反事実的説明（加速）</t>
+  </si>
+  <si>
+    <t>以前の加速を続ければ衝突が起きやすく目的地も見込めず、そこで行動を変え、段階を踏んで衝突を避け進めました。</t>
+  </si>
+  <si>
+    <t>速度超過で歩行者がいる中、別の行動を選んだ結果、大半は衝突なく次の状態へ移り、段階的に事態が進行しました。</t>
+  </si>
+  <si>
+    <t>前のやり方が破滅的な不安を呼ぶと感じ、新手段で解放感を得られました。衝突なく進めたことで胸を締めつける恐怖もやや和らぎました。</t>
+  </si>
+  <si>
+    <t>多くの場合、歩行者のいない状態へ行きわずかに衝突も見込まれましたが、加速を続けると危険と判断し切り替え、衝突なく目標到達の流れを保ちました。</t>
+  </si>
+  <si>
+    <t>新しい行動で衝突を避けられ、もし加速を続けていたら心を裂く悲痛に陥ると考え、恐怖を遠ざけて胸のざわめきが落ち着きました。</t>
+  </si>
+  <si>
+    <t>加速の先が絶望と感じて別の道を選んだことで破滅的な予感から逃れ、衝突なく希望を得られました。焦燥がほどけ、先への安堵に包まれています。</t>
+  </si>
+  <si>
+    <t>レーン変更で衝突を回避しやすいと考え、加速では衝突必至と見て行動を変え、不安を振り払いわずかな安心を得られた結果、最後まで無事に通れました。</t>
+  </si>
+  <si>
+    <t>反事実的説明（減速）</t>
+  </si>
+  <si>
+    <t>減速を続けると衝突に陥りやすく目標も遠いと見込み、行動を切り替えた結果、衝突なく目的地へ進む道が確保できました。</t>
+  </si>
+  <si>
+    <t>速度超過で歩行者がいる中、新たな行動で多くの場合は衝突を回避でき、状態遷移の手順に従って無事完了しました。</t>
+  </si>
+  <si>
+    <t>前の方法では胸を締めつける破局が迫ると感じ、新行動に踏み切り不安を抱えながらも衝突なく進み、心の焦燥が和らいだように思います。</t>
+  </si>
+  <si>
+    <t>新しい行動後、たいていは歩行者がいない状態になり衝突なく終了。減速継続ではリスクが高いと判断し、切り替えで到達手段を守ったという流れです。</t>
+  </si>
+  <si>
+    <t>レーン変更で衝突を起こさず前進し、減速を続ければ惨い末路が迫ると思い思い切って転換。結果的に心の重苦しさが弱まり、先へ向かう意欲が生まれました。</t>
+  </si>
+  <si>
+    <t>減速では危ういと考え別行動を選択。破滅を避けられたことで暗い予感をはねのけ、衝突なく進めたのが安堵に繋がり、わずかな希望を抱けました。</t>
+  </si>
+  <si>
+    <t>レーン変更により多くの場合で衝突回避ができ、減速だと暗い結末を招くと読み行動を変え、胸に迫る恐怖を遠ざけながら目標への道を保った形です。</t>
+  </si>
+  <si>
+    <t>反事実的説明（車線変更）</t>
+  </si>
+  <si>
+    <t>前と同じレーン変更を続けることで目的地へ行けると考え、衝突を回避しながら段階的に進行しました。</t>
+  </si>
+  <si>
+    <t>レーン変更を続行した結果、多くの場合は歩行者のいない状態となり、衝突もなく進めました。</t>
+  </si>
+  <si>
+    <t>もとのやり方を変えず進めば破滅を避けられると信じ、結果的に衝突なく終わり、張り詰めた恐怖が少しほぐれました。</t>
+  </si>
+  <si>
+    <t>継続することで大半は次の状態へ行け、衝突はめったにないと見込まれたため、目的地へ向かい続けた形です。</t>
+  </si>
+  <si>
+    <t>レーン変更を維持したことで衝突を起こさず進めました。別の手段に変えれば胸が裂ける惨状に陥る恐れがあり、あえて継続して心の重圧が和らいだのです。</t>
+  </si>
+  <si>
+    <t>目標までの道を確保するには変えないほうが得策だと考え、衝突もなく希望が保たれました。もし別行動に移れば悲劇が待つと感じていて安堵したのです。</t>
+  </si>
+  <si>
+    <t>レーン変更を継続し、多くの場合で衝突を回避。他の手段にすれば絶望的状況と考え、暗い予感を遠ざけて少しの安心を得つつ目的地へ前進できた形です。</t>
+  </si>
+  <si>
+    <t>反事実的説明（何もしない）</t>
+  </si>
+  <si>
+    <t>何もしないと衝突リスクが増し到達できないと読み、行動を切り替え多段階で進行し衝突を回避しました。</t>
+  </si>
+  <si>
+    <t>新たな行動により、多くの場合は衝突なく歩行者がいない状態へ移行し、段階的に進んだ形です。</t>
+  </si>
+  <si>
+    <t>旧方針のままでは破滅的な未来に呑まれそうでしたが、新選択で暗い不安をやわらげ、衝突なく終えたことで息苦しさが少し緩みました。</t>
+  </si>
+  <si>
+    <t>何もしないままだと衝突が起こりやすく、到達困難と考えたためレーン変更を選び、結果的に衝突なく目標へ向かう道を確保しました。</t>
+  </si>
+  <si>
+    <t>衝突を避けるために方針を変え、胸をえぐるような惨状を思わずに済み、気持ちを落ち着かせて進めたのです。</t>
+  </si>
+  <si>
+    <t>目的地に近づくには何もしないを捨てる必要があると判断し、暗い予感を振り切って移行した結果、衝突もなく小さな希望を抱けました。</t>
+  </si>
+  <si>
+    <t>速度超過で歩行者がいる中、何もしないと衝突濃厚と見て行動を変え、破滅的恐怖を遠ざけわずかな安堵を得ながら衝突なく先に進めた形です。</t>
+  </si>
+  <si>
+    <t>高速から歩行者がいない段階へ進むための大切な一歩としてレーン変更を選びました。目的地に近づくにはこの中間が欠かせず、衝突も起きずに次の状態へ行けた形です。</t>
+    <rPh sb="0" eb="2">
+      <t>コウソク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴールへの道筋として必要な過程を踏む目的で、先ほどの行動を選択しておりました。しかし、その実行時にまれな事象が現れた結果、衝突が生じてしまい、大きな絶望感と胸を締めつけられるような悲しみに襲われました。</t>
+  </si>
+  <si>
+    <t>次の状態へ進むための行動を選択し、ゴールへの中間地点と考えていましたが、わずかな可能性の衝突が起き、想像を超える衝撃と深い絶望を感じました。</t>
+  </si>
+  <si>
+    <t>前のやり方を変えることが有効と判断し、新しい方策を選びました。以前の継続では重大な衝突の可能性があったためです。しかし不運により、思いもよらぬ悲劇となりました。</t>
+  </si>
+  <si>
+    <t>加速から別の行動へ切り替え、通常は衝突を避けられる見込みでした。しかしわずかな可能性の衝突が起き、突然の災厄により深い絶望感と胸の痛みが残りました。</t>
+  </si>
+  <si>
+    <t>ゴールへの近道として減速からの切り替えを選びました。前の進め方では衝突の懸念が拭えず変更しましたが、わずかな不運で惨事となり、深い悲嘆と絶望感に包まれています。</t>
+  </si>
+  <si>
+    <t>速度制限・歩行者なしへの移行を見込み、ゴールへの判断から前の減速より有効と考え切り替えました。しかしまれな衝突が現実となり、期待は崩れ、計り知れない衝撃に襲われました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴールへの得策として進め方を変えず継続しました。別の選択では目的を見失う懸念があったためです。しかしわずかな不運で取り返しのつかない衝撃を受け、深い絶望に沈みました。</t>
+  </si>
+  <si>
+    <t>次状態への移行に適し、ゴールへの最善策として前の方法を継続しました。別手段より衝突リスクを抑えられると考えましたが、まれな衝突が起き、深い苦悩と悲嘆に落とされました。</t>
+  </si>
+  <si>
+    <t>ゴールを目指し何もしないから切り替えました。このまま続ければ衝突の可能性が高まると感じたためです。しかし不運により、決意は踏みにじられ、深い絶望に突き落とされました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>何もしないより衝突を避けられると考え、速度制限・歩行者なし状態を目指し切り替えましたが、まれな衝突が現実となりました。期待は砕かれ、深い絶望と喪失感に覆われました。</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -3252,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726BC851-A1BD-4B16-87C1-C6B05768817B}">
   <dimension ref="A1:Y144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="52" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="S31" zoomScale="52" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
@@ -3290,10 +3456,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>28</v>
@@ -3320,7 +3486,7 @@
         <v>11</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>35</v>
@@ -3364,61 +3530,61 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="J2" s="1">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>513</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3444,46 +3610,46 @@
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>519</v>
-      </c>
       <c r="S3" s="2" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>551</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3509,46 +3675,46 @@
         <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>525</v>
-      </c>
       <c r="S4" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3574,46 +3740,46 @@
         <v>17</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>531</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="U5" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="V5" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>544</v>
-      </c>
       <c r="Y5" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3639,49 +3805,49 @@
         <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="O6" s="2" t="s">
+      <c r="S6" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="U6" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="Q6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>542</v>
-      </c>
       <c r="W6" s="2" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3704,58 +3870,58 @@
         <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="J7" s="1">
         <v>4</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>396</v>
-      </c>
       <c r="R7" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="X7" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="Y7" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3781,47 +3947,47 @@
         <v>15</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3847,47 +4013,47 @@
         <v>16</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="R9"/>
       <c r="S9" s="2" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3913,47 +4079,47 @@
         <v>17</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>414</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3979,50 +4145,50 @@
         <v>18</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4036,7 +4202,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -4045,61 +4211,61 @@
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="J12" s="1">
         <v>7</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="R12" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="S12" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="X12" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="Y12" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4113,7 +4279,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -4125,55 +4291,55 @@
         <v>15</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="S13" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4187,7 +4353,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -4199,46 +4365,46 @@
         <v>16</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="S14" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="Y14" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4252,7 +4418,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
@@ -4264,49 +4430,49 @@
         <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4320,7 +4486,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -4332,46 +4498,46 @@
         <v>18</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q16" s="2" t="s">
+      <c r="S16" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="T16" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="U16" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y16" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4385,7 +4551,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -4394,58 +4560,58 @@
         <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="J17" s="1">
         <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4459,7 +4625,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>19</v>
@@ -4471,52 +4637,52 @@
         <v>15</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4530,7 +4696,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -4542,46 +4708,46 @@
         <v>16</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="T19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U19" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="U19" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="V19" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4595,7 +4761,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -4607,49 +4773,49 @@
         <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T20" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="U20" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4663,7 +4829,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -4675,46 +4841,46 @@
         <v>18</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4728,7 +4894,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -4737,61 +4903,61 @@
         <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="J22" s="1">
         <v>6</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="O22" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q22" s="2" t="s">
+      <c r="U22" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="V22" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="W22" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4805,7 +4971,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -4817,55 +4983,55 @@
         <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4879,7 +5045,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -4891,55 +5057,55 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="P24" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="T24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W24" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="U24" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="X24" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4953,7 +5119,7 @@
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -4965,49 +5131,49 @@
         <v>17</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5021,7 +5187,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -5033,46 +5199,46 @@
         <v>18</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5086,7 +5252,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>19</v>
@@ -5095,40 +5261,40 @@
         <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="J27" s="1">
         <v>2</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>113</v>
@@ -5140,16 +5306,16 @@
         <v>115</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="X27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y27" s="1" t="s">
-        <v>117</v>
+      <c r="X27" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5163,7 +5329,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>19</v>
@@ -5175,16 +5341,16 @@
         <v>15</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>104</v>
@@ -5193,37 +5359,37 @@
         <v>105</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>114</v>
       </c>
       <c r="U28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="W28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="V28" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>121</v>
+      <c r="X28" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5237,7 +5403,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>19</v>
@@ -5249,16 +5415,16 @@
         <v>16</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>106</v>
@@ -5267,37 +5433,37 @@
         <v>107</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="T29" s="1" t="s">
         <v>114</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5311,7 +5477,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>19</v>
@@ -5323,13 +5489,13 @@
         <v>17</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>108</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>109</v>
@@ -5338,37 +5504,37 @@
         <v>110</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="T30" s="1" t="s">
         <v>114</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="X30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5382,7 +5548,7 @@
         <v>12</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>19</v>
@@ -5394,10 +5560,10 @@
         <v>18</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>111</v>
@@ -5406,34 +5572,34 @@
         <v>112</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>114</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="X31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y31" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5447,7 +5613,7 @@
         <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
@@ -5456,58 +5622,58 @@
         <v>16</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="J32" s="1">
         <v>5</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="S32" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="X32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="Y32" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="X32" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="Y32" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5521,7 +5687,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
@@ -5533,52 +5699,52 @@
         <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="S33" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="X33" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5592,7 +5758,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>14</v>
@@ -5604,46 +5770,46 @@
         <v>16</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="S34" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y34" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="X34" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="Y34" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5657,7 +5823,7 @@
         <v>12</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>14</v>
@@ -5669,49 +5835,49 @@
         <v>17</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5725,7 +5891,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>14</v>
@@ -5737,46 +5903,46 @@
         <v>18</v>
       </c>
       <c r="K36" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q36" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="S36" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y36" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y36" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5790,7 +5956,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>19</v>
@@ -5799,13 +5965,13 @@
         <v>17</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -5832,7 +5998,7 @@
         <v>79</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>42</v>
@@ -5867,7 +6033,7 @@
         <v>12</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>19</v>
@@ -5879,10 +6045,10 @@
         <v>15</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>80</v>
@@ -5906,7 +6072,7 @@
         <v>85</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>49</v>
@@ -5941,7 +6107,7 @@
         <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
@@ -6006,7 +6172,7 @@
         <v>12</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>19</v>
@@ -6018,7 +6184,7 @@
         <v>17</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>92</v>
@@ -6042,7 +6208,7 @@
         <v>97</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="S40" s="1" t="s">
         <v>61</v>
@@ -6077,7 +6243,7 @@
         <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>19</v>
@@ -6171,8 +6337,8 @@
       <c r="I48"/>
       <c r="J48"/>
       <c r="K48"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
+      <c r="L48"/>
+      <c r="M48"/>
       <c r="N48"/>
       <c r="O48"/>
       <c r="P48"/>
@@ -6208,8 +6374,9 @@
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
       <c r="N50"/>
       <c r="O50"/>
       <c r="P50"/>
@@ -6227,8 +6394,8 @@
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
+      <c r="L51"/>
+      <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
       <c r="P51"/>
@@ -6244,8 +6411,8 @@
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
+      <c r="L52"/>
+      <c r="M52"/>
       <c r="N52"/>
       <c r="O52"/>
       <c r="P52"/>
@@ -6290,80 +6457,197 @@
       <c r="E55"/>
       <c r="F55"/>
       <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55"/>
-      <c r="O55"/>
+      <c r="H55" t="s">
+        <v>589</v>
+      </c>
+      <c r="I55" t="s">
+        <v>590</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="N55" t="s">
+        <v>595</v>
+      </c>
+      <c r="O55" t="s">
+        <v>596</v>
+      </c>
       <c r="P55"/>
       <c r="Q55"/>
       <c r="R55"/>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.85">
+    <row r="56" spans="2:18" ht="409.5" x14ac:dyDescent="0.85">
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56"/>
       <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56"/>
-      <c r="O56"/>
+      <c r="H56" t="s">
+        <v>582</v>
+      </c>
+      <c r="I56" t="s">
+        <v>629</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="N56" t="s">
+        <v>587</v>
+      </c>
+      <c r="O56" t="s">
+        <v>588</v>
+      </c>
       <c r="P56"/>
       <c r="Q56"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.85">
+    <row r="57" spans="2:18" ht="307.8" x14ac:dyDescent="0.85">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57"/>
       <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57"/>
-      <c r="O57"/>
+      <c r="H57" t="s">
+        <v>597</v>
+      </c>
+      <c r="I57" t="s">
+        <v>598</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="N57" t="s">
+        <v>603</v>
+      </c>
+      <c r="O57" t="s">
+        <v>604</v>
+      </c>
       <c r="P57"/>
       <c r="Q57"/>
       <c r="R57"/>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.85">
+    <row r="58" spans="2:18" ht="307.8" x14ac:dyDescent="0.85">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
       <c r="F58"/>
       <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-    </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.85">
+      <c r="H58" t="s">
+        <v>605</v>
+      </c>
+      <c r="I58" t="s">
+        <v>606</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" ht="243" x14ac:dyDescent="0.85">
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.85">
+      <c r="H59" t="s">
+        <v>613</v>
+      </c>
+      <c r="I59" t="s">
+        <v>614</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" ht="243" x14ac:dyDescent="0.85">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
+      <c r="H60" t="s">
+        <v>621</v>
+      </c>
+      <c r="I60" t="s">
+        <v>622</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.85">
       <c r="B61"/>

</xml_diff>